<commit_message>
add and fix user import
</commit_message>
<xml_diff>
--- a/Scanorders2/src/Oleg/UserdirectoryBundle/Util/UsersFullShort.xlsx
+++ b/Scanorders2/src/Oleg/UserdirectoryBundle/Util/UsersFullShort.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="51195" windowHeight="24240"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="51195" windowHeight="24180"/>
   </bookViews>
   <sheets>
     <sheet name="owssvr.dll" sheetId="1" r:id="rId1"/>
@@ -14,11 +14,6 @@
     <definedName name="Work" localSheetId="0">owssvr.dll!#REF!</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -31,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="310">
   <si>
     <t>A</t>
   </si>
@@ -829,6 +824,138 @@
   </si>
   <si>
     <t>lhellens@med.cornell.edu</t>
+  </si>
+  <si>
+    <t>D'Alfonso</t>
+  </si>
+  <si>
+    <t>Timothy</t>
+  </si>
+  <si>
+    <t>Assistant Attending Pathologist</t>
+  </si>
+  <si>
+    <t>Assistant Professor of Pathology and Laboratory Medicine</t>
+  </si>
+  <si>
+    <t>7/16/2012</t>
+  </si>
+  <si>
+    <t>(212) 746-6393</t>
+  </si>
+  <si>
+    <t>(212) 746-6484</t>
+  </si>
+  <si>
+    <t>(212) 746-6700 16295</t>
+  </si>
+  <si>
+    <t>Starr-1031E</t>
+  </si>
+  <si>
+    <t>tid9007@med.cornell.edu</t>
+  </si>
+  <si>
+    <t>tid9007</t>
+  </si>
+  <si>
+    <t>7/29/2011</t>
+  </si>
+  <si>
+    <t>12/31/2021</t>
+  </si>
+  <si>
+    <t>7236D</t>
+  </si>
+  <si>
+    <t>260165</t>
+  </si>
+  <si>
+    <t>1699938324; 200-33-580</t>
+  </si>
+  <si>
+    <t>http://www.weillcornell.org/physician/tdalfonso/index.html</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/pubmed?term=D%27Alfonso%20TM%5BAuthor%5D</t>
+  </si>
+  <si>
+    <t>http://vivo.med.cornell.edu/display/cwid-tid9007</t>
+  </si>
+  <si>
+    <t>Hoda</t>
+  </si>
+  <si>
+    <t>Syed</t>
+  </si>
+  <si>
+    <t>Education Coordinator, Anatomic Pathology</t>
+  </si>
+  <si>
+    <t>Professor of Clinical Pathology &amp; Laboratory Medicine</t>
+  </si>
+  <si>
+    <t>7/1/1992</t>
+  </si>
+  <si>
+    <t>(212) 746-2708</t>
+  </si>
+  <si>
+    <t>(212) 746-6700 17617</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Starr-1031C</t>
+  </si>
+  <si>
+    <t>sahoda@med.cornell.edu</t>
+  </si>
+  <si>
+    <t>sahoda</t>
+  </si>
+  <si>
+    <t>Anatomic Pathology/Clinical Pathology; Cytopathology</t>
+  </si>
+  <si>
+    <t>8/30/1990; 6/4/1991</t>
+  </si>
+  <si>
+    <t>null; 1/1/2022</t>
+  </si>
+  <si>
+    <t>null; 1/1/2012</t>
+  </si>
+  <si>
+    <t>HO079</t>
+  </si>
+  <si>
+    <t>182096-1</t>
+  </si>
+  <si>
+    <t>1/31/2016</t>
+  </si>
+  <si>
+    <t>1346280583; 200-18-968</t>
+  </si>
+  <si>
+    <t>HODAS1</t>
+  </si>
+  <si>
+    <t>CQP79473</t>
+  </si>
+  <si>
+    <t>10/2/2016</t>
+  </si>
+  <si>
+    <t>http://www.cornellphysicians.com/shoda</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/pubmed?term=Hoda%20SA%5BAuthor%5D</t>
+  </si>
+  <si>
+    <t>http://vivo.med.cornell.edu/display/cwid-sahoda</t>
   </si>
 </sst>
 </file>
@@ -1635,7 +1762,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1739,6 +1866,44 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="288">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2035,18 +2200,6 @@
       <font>
         <color auto="1"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
@@ -2196,6 +2349,13 @@
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
@@ -2921,9 +3081,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2936,15 +3101,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr.dll" displayName="Table_owssvr.dll" ref="A1:BL4" totalsRowShown="0" headerRowDxfId="65" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr.dll" displayName="Table_owssvr.dll" ref="A1:BL4" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
   <autoFilter ref="A1:BL4"/>
   <sortState ref="A2:BL356">
     <sortCondition ref="D1:D356"/>
@@ -3003,17 +3165,17 @@
     <tableColumn id="49" name="Administrative Comment - Name" dataDxfId="13"/>
     <tableColumn id="50" name="Administrative Comment - Comment" dataDxfId="12"/>
     <tableColumn id="51" name="Identifier - Type" dataDxfId="11"/>
-    <tableColumn id="52" name="Identifier" dataDxfId="64"/>
-    <tableColumn id="53" name="Identifier - link" dataDxfId="10"/>
-    <tableColumn id="55" name="Certificate of Qualification - Code" dataDxfId="9"/>
-    <tableColumn id="56" name="Certificate of Qualification - Serial Number" dataDxfId="8"/>
-    <tableColumn id="57" name="Certificate of Qualification - Expiration Date" dataDxfId="7"/>
-    <tableColumn id="59" name="CLIA - Number" dataDxfId="6"/>
-    <tableColumn id="58" name="CLIA - Expiration Date" dataDxfId="5"/>
-    <tableColumn id="60" name="PFI" dataDxfId="4"/>
-    <tableColumn id="68" name="POPS Link" dataDxfId="3"/>
-    <tableColumn id="70" name="Pubmed Link" dataDxfId="2"/>
-    <tableColumn id="69" name="VIVO link" dataDxfId="1"/>
+    <tableColumn id="52" name="Identifier" dataDxfId="10"/>
+    <tableColumn id="53" name="Identifier - link" dataDxfId="9"/>
+    <tableColumn id="55" name="Certificate of Qualification - Code" dataDxfId="8"/>
+    <tableColumn id="56" name="Certificate of Qualification - Serial Number" dataDxfId="7"/>
+    <tableColumn id="57" name="Certificate of Qualification - Expiration Date" dataDxfId="6"/>
+    <tableColumn id="59" name="CLIA - Number" dataDxfId="5"/>
+    <tableColumn id="58" name="CLIA - Expiration Date" dataDxfId="4"/>
+    <tableColumn id="60" name="PFI" dataDxfId="3"/>
+    <tableColumn id="68" name="POPS Link" dataDxfId="2"/>
+    <tableColumn id="70" name="Pubmed Link" dataDxfId="1"/>
+    <tableColumn id="69" name="VIVO link" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3274,7 +3436,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3282,12 +3444,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BU11"/>
+  <dimension ref="A1:BU13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="AH1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="AG1" activePane="topRight" state="frozen"/>
       <selection activeCell="C89" sqref="C89"/>
-      <selection pane="topRight" activeCell="AC11" sqref="AC11"/>
+      <selection pane="topRight" activeCell="AO9" sqref="AO1:AO1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3328,6 +3490,7 @@
     <col min="38" max="38" width="14" style="11" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="16" style="11" customWidth="1"/>
     <col min="40" max="40" width="17.28515625" style="11" customWidth="1"/>
+    <col min="41" max="41" width="22.85546875" customWidth="1"/>
     <col min="43" max="43" width="21.85546875" style="11" customWidth="1"/>
     <col min="44" max="44" width="30.140625" style="11" customWidth="1"/>
     <col min="45" max="45" width="21.85546875" style="11" customWidth="1"/>
@@ -4910,6 +5073,292 @@
       <c r="BT11" s="10"/>
       <c r="BU11" s="10"/>
     </row>
+    <row r="12" spans="1:73" ht="60">
+      <c r="C12" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>266</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="I12" s="42"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="R12" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="S12" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="T12" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="U12" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="V12" s="38"/>
+      <c r="W12" s="38"/>
+      <c r="X12" s="38"/>
+      <c r="Y12" s="42" t="s">
+        <v>269</v>
+      </c>
+      <c r="Z12" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="AA12" s="38" t="s">
+        <v>270</v>
+      </c>
+      <c r="AB12" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC12" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD12" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE12" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF12" s="38"/>
+      <c r="AG12" s="38"/>
+      <c r="AH12" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="AI12" s="38" t="s">
+        <v>272</v>
+      </c>
+      <c r="AJ12" s="38" t="s">
+        <v>273</v>
+      </c>
+      <c r="AK12" s="38"/>
+      <c r="AL12" s="38" t="s">
+        <v>274</v>
+      </c>
+      <c r="AM12" s="38" t="s">
+        <v>275</v>
+      </c>
+      <c r="AN12" s="38" t="s">
+        <v>276</v>
+      </c>
+      <c r="AO12" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP12" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="AQ12" s="38" t="s">
+        <v>278</v>
+      </c>
+      <c r="AR12" s="38"/>
+      <c r="AS12" s="38" t="s">
+        <v>279</v>
+      </c>
+      <c r="AT12" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="AU12" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="AV12" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="AW12" s="38"/>
+      <c r="AX12" s="38"/>
+      <c r="AY12" s="38"/>
+      <c r="AZ12" s="38"/>
+      <c r="BA12" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="BB12" s="37" t="s">
+        <v>281</v>
+      </c>
+      <c r="BC12" s="38"/>
+      <c r="BD12" s="38"/>
+      <c r="BE12" s="38"/>
+      <c r="BF12" s="38"/>
+      <c r="BG12" s="38"/>
+      <c r="BH12" s="40"/>
+      <c r="BI12" s="40"/>
+      <c r="BJ12" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="BK12" s="40" t="s">
+        <v>283</v>
+      </c>
+      <c r="BL12" s="40" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="13" spans="1:73" ht="135">
+      <c r="C13" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="45" t="s">
+        <v>285</v>
+      </c>
+      <c r="E13" s="45" t="s">
+        <v>286</v>
+      </c>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="H13" s="46" t="s">
+        <v>172</v>
+      </c>
+      <c r="I13" s="49" t="s">
+        <v>287</v>
+      </c>
+      <c r="J13" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="K13" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="L13" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="M13" s="45"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="45"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="R13" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="S13" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="T13" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="U13" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="V13" s="44"/>
+      <c r="W13" s="45"/>
+      <c r="X13" s="45"/>
+      <c r="Y13" s="50" t="s">
+        <v>288</v>
+      </c>
+      <c r="Z13" s="45" t="s">
+        <v>226</v>
+      </c>
+      <c r="AA13" s="45" t="s">
+        <v>289</v>
+      </c>
+      <c r="AB13" s="48" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC13" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD13" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE13" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF13" s="45"/>
+      <c r="AG13" s="45"/>
+      <c r="AH13" s="45" t="s">
+        <v>290</v>
+      </c>
+      <c r="AI13" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ13" s="45" t="s">
+        <v>291</v>
+      </c>
+      <c r="AK13" s="45" t="s">
+        <v>292</v>
+      </c>
+      <c r="AL13" s="45" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM13" s="45" t="s">
+        <v>294</v>
+      </c>
+      <c r="AN13" s="45" t="s">
+        <v>295</v>
+      </c>
+      <c r="AO13" s="45" t="s">
+        <v>296</v>
+      </c>
+      <c r="AP13" s="45" t="s">
+        <v>297</v>
+      </c>
+      <c r="AQ13" s="45" t="s">
+        <v>298</v>
+      </c>
+      <c r="AR13" s="45" t="s">
+        <v>299</v>
+      </c>
+      <c r="AS13" s="45" t="s">
+        <v>300</v>
+      </c>
+      <c r="AT13" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="AU13" s="45" t="s">
+        <v>301</v>
+      </c>
+      <c r="AV13" s="45" t="s">
+        <v>302</v>
+      </c>
+      <c r="AW13" s="45"/>
+      <c r="AX13" s="45"/>
+      <c r="AY13" s="45"/>
+      <c r="AZ13" s="45"/>
+      <c r="BA13" s="45" t="s">
+        <v>185</v>
+      </c>
+      <c r="BB13" s="43" t="s">
+        <v>303</v>
+      </c>
+      <c r="BC13" s="45"/>
+      <c r="BD13" s="45" t="s">
+        <v>304</v>
+      </c>
+      <c r="BE13" s="45" t="s">
+        <v>305</v>
+      </c>
+      <c r="BF13" s="45" t="s">
+        <v>306</v>
+      </c>
+      <c r="BG13" s="45"/>
+      <c r="BH13" s="47"/>
+      <c r="BI13" s="47"/>
+      <c r="BJ13" s="47" t="s">
+        <v>307</v>
+      </c>
+      <c r="BK13" s="47" t="s">
+        <v>308</v>
+      </c>
+      <c r="BL13" s="47" t="s">
+        <v>309</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="AM8" r:id="rId1"/>
@@ -4921,10 +5370,5 @@
   <tableParts count="1">
     <tablePart r:id="rId5"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>